<commit_message>
platform stm32f4: update function mappings
</commit_message>
<xml_diff>
--- a/platform/stm32f407/stm32f4_function_mappings.xlsx
+++ b/platform/stm32f407/stm32f4_function_mappings.xlsx
@@ -1689,27 +1689,29 @@
   <dimension ref="A1:Q142"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Q17" activeCellId="0" sqref="Q17"/>
+      <selection pane="bottomLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="bottomRight" activeCell="I22" activeCellId="0" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.7448979591837"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="14.1020408163265"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.265306122449"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.7040816326531"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2342,7 +2344,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="8" t="s">
         <v>93</v>
       </c>
@@ -2395,7 +2397,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="8" t="s">
         <v>98</v>
       </c>
@@ -2448,7 +2450,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="8" t="s">
         <v>103</v>
       </c>
@@ -2972,105 +2974,105 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="5" t="s">
+    <row r="25" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="B25" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D25" s="6" t="s">
+      <c r="B25" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="E25" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F25" s="6" t="s">
+      <c r="E25" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F25" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="G25" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="H25" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="I25" s="6" t="s">
+      <c r="G25" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H25" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="I25" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="J25" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="K25" s="6" t="s">
+      <c r="J25" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="K25" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="L25" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="M25" s="6"/>
-      <c r="N25" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="O25" s="6" t="s">
+      <c r="L25" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="O25" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="P25" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q25" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="5" t="s">
+      <c r="P25" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q25" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="B26" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D26" s="6" t="s">
+      <c r="B26" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="E26" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F26" s="6" t="s">
+      <c r="E26" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F26" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="G26" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="H26" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="I26" s="6" t="s">
+      <c r="G26" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="I26" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="J26" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="K26" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="L26" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="M26" s="6"/>
-      <c r="N26" s="6" t="s">
+      <c r="J26" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="K26" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="L26" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="M26" s="9"/>
+      <c r="N26" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="O26" s="0" t="s">
+      <c r="O26" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="P26" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q26" s="6" t="s">
+      <c r="P26" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q26" s="9" t="s">
         <v>32</v>
       </c>
     </row>
@@ -3867,7 +3869,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="42" s="23" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="19" t="s">
         <v>216</v>
       </c>
@@ -4026,7 +4028,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="45" s="27" customFormat="true" ht="25.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="25.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="24" t="s">
         <v>233</v>
       </c>
@@ -4079,7 +4081,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="46" s="27" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="24" t="s">
         <v>237</v>
       </c>
@@ -4132,7 +4134,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="47" s="27" customFormat="true" ht="25.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="25.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="24" t="s">
         <v>240</v>
       </c>
@@ -4768,7 +4770,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="59" s="33" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="30" t="s">
         <v>266</v>
       </c>
@@ -4821,7 +4823,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="60" s="33" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="30" t="s">
         <v>268</v>
       </c>
@@ -4874,7 +4876,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="61" s="33" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="30" t="s">
         <v>270</v>
       </c>
@@ -4927,7 +4929,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="62" s="33" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="30" t="s">
         <v>272</v>
       </c>
@@ -5033,56 +5035,56 @@
         <v>32</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="5" t="s">
+    <row r="64" s="37" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="35" t="s">
         <v>276</v>
       </c>
-      <c r="B64" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C64" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D64" s="6" t="s">
+      <c r="B64" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="C64" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="D64" s="36" t="s">
         <v>149</v>
       </c>
-      <c r="E64" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F64" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G64" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="H64" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="I64" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="J64" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="K64" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="L64" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="M64" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="N64" s="6" t="s">
+      <c r="E64" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="F64" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="G64" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="H64" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="I64" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="J64" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="K64" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="L64" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="M64" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="N64" s="36" t="s">
         <v>277</v>
       </c>
-      <c r="O64" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="P64" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q64" s="6" t="s">
+      <c r="O64" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="P64" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q64" s="36" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>